<commit_message>
Improvement of results in (restraining parameters->Omegam_OmegaL) and removal of pdfs of articles in order to put them into Zotero
</commit_message>
<xml_diff>
--- a/1_analyse données Pantheon +/restraining parameters/résultats_CL_68_param_cosmo(à compléter).xlsx
+++ b/1_analyse données Pantheon +/restraining parameters/résultats_CL_68_param_cosmo(à compléter).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emile\Desktop\Supaero 3A 2023-2024\projet recherche\travail concret projet\1_analyse données Pantheon +\restraining parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emile\Desktop\Supaero_3A_2023-2024\projet_recherche\travail_concret_projet\1_analyse données Pantheon +\restraining parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454BA707-B37A-4AE2-877E-3EE6CD3B8DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3A17DA-240B-4329-92B9-A2D02CD0D9D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,9 +40,11 @@
   <authors>
     <author>tc={15528B95-39C7-4CC7-902A-00229DEA6DB7}</author>
     <author>tc={AF607B9B-BC83-4D48-8FD5-844F9B258B2E}</author>
+    <author>tc={176F64C0-3E19-43A0-A9B6-591B40052657}</author>
+    <author>tc={53E0E4B3-50BA-4E72-B223-0D1D050D6508}</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{15528B95-39C7-4CC7-902A-00229DEA6DB7}">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{15528B95-39C7-4CC7-902A-00229DEA6DB7}">
       <text>
         <t>[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
@@ -50,7 +52,7 @@
      (sans doute minimisé car range trop petit (s'arrête à 75))</t>
       </text>
     </comment>
-    <comment ref="G2" authorId="1" shapeId="0" xr:uid="{AF607B9B-BC83-4D48-8FD5-844F9B258B2E}">
+    <comment ref="G3" authorId="1" shapeId="0" xr:uid="{AF607B9B-BC83-4D48-8FD5-844F9B258B2E}">
       <text>
         <t>[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
@@ -58,12 +60,28 @@
     Meilleure précision que le papier de Brout ! &lt;- cache quelque chose ...</t>
       </text>
     </comment>
+    <comment ref="F4" authorId="2" shapeId="0" xr:uid="{176F64C0-3E19-43A0-A9B6-591B40052657}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    (sans doute minimisé car range trop petit (s'arrête à 0.35))</t>
+      </text>
+    </comment>
+    <comment ref="K4" authorId="3" shapeId="0" xr:uid="{53E0E4B3-50BA-4E72-B223-0D1D050D6508}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    Min de chi2 très similaire à celui pour Omegam_H0 : pourrait être utilisé comme référence pour la suite pour voir si les modèles avec les G(z) améliorent ou non les fits</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>+</t>
   </si>
@@ -90,6 +108,12 @@
   </si>
   <si>
     <t>Omegam_H0 (pour LambdaCDM)</t>
+  </si>
+  <si>
+    <t>Omegam_Omegal(pour LambdaCDM)</t>
+  </si>
+  <si>
+    <t>Résultats attendus pour Flat LCDM (Brout et al. 2022)</t>
   </si>
 </sst>
 </file>
@@ -435,11 +459,17 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="C2" dT="2023-12-18T09:19:56.88" personId="{5B684DBE-077F-44CE-8336-DBD6409E8451}" id="{15528B95-39C7-4CC7-902A-00229DEA6DB7}">
+  <threadedComment ref="C3" dT="2023-12-18T09:19:56.88" personId="{5B684DBE-077F-44CE-8336-DBD6409E8451}" id="{15528B95-39C7-4CC7-902A-00229DEA6DB7}">
     <text xml:space="preserve"> (sans doute minimisé car range trop petit (s'arrête à 75))</text>
   </threadedComment>
-  <threadedComment ref="G2" dT="2023-12-12T13:12:57.39" personId="{5B684DBE-077F-44CE-8336-DBD6409E8451}" id="{AF607B9B-BC83-4D48-8FD5-844F9B258B2E}">
+  <threadedComment ref="G3" dT="2023-12-12T13:12:57.39" personId="{5B684DBE-077F-44CE-8336-DBD6409E8451}" id="{AF607B9B-BC83-4D48-8FD5-844F9B258B2E}">
     <text>Meilleure précision que le papier de Brout ! &lt;- cache quelque chose ...</text>
+  </threadedComment>
+  <threadedComment ref="F4" dT="2023-12-27T14:11:34.34" personId="{5B684DBE-077F-44CE-8336-DBD6409E8451}" id="{176F64C0-3E19-43A0-A9B6-591B40052657}">
+    <text>(sans doute minimisé car range trop petit (s'arrête à 0.35))</text>
+  </threadedComment>
+  <threadedComment ref="K4" dT="2023-12-27T14:18:31.21" personId="{5B684DBE-077F-44CE-8336-DBD6409E8451}" id="{53E0E4B3-50BA-4E72-B223-0D1D050D6508}">
+    <text>Min de chi2 très similaire à celui pour Omegam_H0 : pourrait être utilisé comme référence pour la suite pour voir si les modèles avec les G(z) améliorent ou non les fits</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -449,12 +479,12 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="1" max="1" width="50" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="21.140625" customWidth="1"/>
     <col min="8" max="8" width="18.42578125" customWidth="1"/>
@@ -504,39 +534,108 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="C2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E2">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="F2">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="G2">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="H2">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="I2">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="J2">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>73.2999999999995</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>1.7</v>
       </c>
-      <c r="D2">
-        <f>ABS(B2-(69.5999999999997))</f>
+      <c r="D3">
+        <f>ABS(B3-(69.5999999999997))</f>
         <v>3.6999999999998039</v>
       </c>
-      <c r="E2">
+      <c r="E3">
         <f>33.4000000000001/100</f>
         <v>0.33400000000000096</v>
       </c>
-      <c r="F2">
-        <f>ABS(E2-(35.0000000000001/100))</f>
+      <c r="F3">
+        <f>ABS(E3-(35.0000000000001/100))</f>
         <v>1.6000000000000014E-2</v>
       </c>
-      <c r="G2">
-        <f>ABS(E2-(32.5000000000001/100))</f>
+      <c r="G3">
+        <f>ABS(E3-(32.5000000000001/100))</f>
         <v>8.9999999999999525E-3</v>
       </c>
-      <c r="K2">
+      <c r="K3">
         <v>1523.01688482443</v>
       </c>
-      <c r="L2">
+      <c r="L3">
         <v>2</v>
       </c>
-      <c r="M2">
-        <f>K2+2*L2</f>
+      <c r="M3">
+        <f>K3+2*L3</f>
         <v>1527.01688482443</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>0.33</v>
+      </c>
+      <c r="F4">
+        <f>ABS(E4-0.35)</f>
+        <v>1.9999999999999962E-2</v>
+      </c>
+      <c r="G4">
+        <f>ABS(E4-0.306)</f>
+        <v>2.4000000000000021E-2</v>
+      </c>
+      <c r="H4">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="I4">
+        <f>ABS(H4-0.694)</f>
+        <v>3.1999999999999917E-2</v>
+      </c>
+      <c r="J4">
+        <f>ABS(H4-0.633)</f>
+        <v>2.9000000000000026E-2</v>
+      </c>
+      <c r="K4">
+        <v>1523.01055414283</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <f>K4+2*L4</f>
+        <v>1527.01055414283</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
new plots of resuduals + update OmegaM_w + creation of ppt 'Récapitulatif chi2,HD,résidus'
</commit_message>
<xml_diff>
--- a/1_analyse données Pantheon +/restraining parameters/résultats_CL_68_param_cosmo(à compléter).xlsx
+++ b/1_analyse données Pantheon +/restraining parameters/résultats_CL_68_param_cosmo(à compléter).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emile\Desktop\Supaero_3A_2023-2024\projet_recherche\travail_concret_projet\1_analyse données Pantheon +\restraining parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3A17DA-240B-4329-92B9-A2D02CD0D9D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C22F573-5F52-47C2-8829-D7313F1EB1CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,6 +42,7 @@
     <author>tc={AF607B9B-BC83-4D48-8FD5-844F9B258B2E}</author>
     <author>tc={176F64C0-3E19-43A0-A9B6-591B40052657}</author>
     <author>tc={53E0E4B3-50BA-4E72-B223-0D1D050D6508}</author>
+    <author>Emile DOSSO</author>
   </authors>
   <commentList>
     <comment ref="C3" authorId="0" shapeId="0" xr:uid="{15528B95-39C7-4CC7-902A-00229DEA6DB7}">
@@ -76,12 +77,37 @@
     Min de chi2 très similaire à celui pour Omegam_H0 : pourrait être utilisé comme référence pour la suite pour voir si les modèles avec les G(z) améliorent ou non les fits</t>
       </text>
     </comment>
+    <comment ref="G8" authorId="4" shapeId="0" xr:uid="{EB0C4327-299A-426F-82A7-303506DA3CE8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Emile DOSSO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+étonamment précis en comparaison aux résultats de Brout…
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>+</t>
   </si>
@@ -114,13 +140,31 @@
   </si>
   <si>
     <t>Résultats attendus pour Flat LCDM (Brout et al. 2022)</t>
+  </si>
+  <si>
+    <t>Résultats attendus pour Flat wCDM (Brout et al. 2022)</t>
+  </si>
+  <si>
+    <t>Omegam_w(pour flat wCDM)</t>
+  </si>
+  <si>
+    <t>(w=-0,90) 0,691</t>
+  </si>
+  <si>
+    <t>(0,14 pour w) 0,069</t>
+  </si>
+  <si>
+    <t>(0,14 pour w) -0,063</t>
+  </si>
+  <si>
+    <t>range trop restreint</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,24 +173,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="4" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -169,10 +206,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,7 +515,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,7 +524,8 @@
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="21.140625" customWidth="1"/>
     <col min="8" max="8" width="18.42578125" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" customWidth="1"/>
+    <col min="10" max="10" width="21.28515625" customWidth="1"/>
     <col min="11" max="11" width="27" customWidth="1"/>
     <col min="12" max="12" width="21.5703125" customWidth="1"/>
     <col min="13" max="13" width="10.28515625" customWidth="1"/>
@@ -639,13 +676,65 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>73.5</v>
+      </c>
+      <c r="C7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E7">
+        <v>0.309</v>
+      </c>
+      <c r="F7">
+        <v>6.3E-2</v>
+      </c>
+      <c r="G7">
+        <v>-6.9000000000000006E-2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="F8">
+        <f>ABS(E8-0.308)</f>
+        <v>7.0000000000000062E-3</v>
+      </c>
+      <c r="G8">
+        <f>ABS(E8-0.29)</f>
+        <v>1.100000000000001E-2</v>
+      </c>
+      <c r="H8">
+        <v>-0.92</v>
+      </c>
+      <c r="I8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
implementation of only alpha_fixé_H0_Omegam in 'Mesure uniquement' + modification of some program in 'restraining parameters'
</commit_message>
<xml_diff>
--- a/1_analyse données Pantheon +/restraining parameters/résultats_CL_68_param_cosmo(à compléter).xlsx
+++ b/1_analyse données Pantheon +/restraining parameters/résultats_CL_68_param_cosmo(à compléter).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emile\Desktop\Supaero_3A_2023-2024\projet_recherche\travail_concret_projet\1_analyse données Pantheon +\restraining parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C22F573-5F52-47C2-8829-D7313F1EB1CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D328114C-2253-40FB-A432-84EC6F761D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,7 +77,7 @@
     Min de chi2 très similaire à celui pour Omegam_H0 : pourrait être utilisé comme référence pour la suite pour voir si les modèles avec les G(z) améliorent ou non les fits</t>
       </text>
     </comment>
-    <comment ref="G8" authorId="4" shapeId="0" xr:uid="{EB0C4327-299A-426F-82A7-303506DA3CE8}">
+    <comment ref="G10" authorId="4" shapeId="0" xr:uid="{EB0C4327-299A-426F-82A7-303506DA3CE8}">
       <text>
         <r>
           <rPr>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>+</t>
   </si>
@@ -158,6 +158,15 @@
   </si>
   <si>
     <t>range trop restreint</t>
+  </si>
+  <si>
+    <t>H0fixé_Omegamrecherche</t>
+  </si>
+  <si>
+    <t>1-0,314 = 0,686</t>
+  </si>
+  <si>
+    <t>Omegamfixé_H0recherche</t>
   </si>
 </sst>
 </file>
@@ -512,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,60 +684,123 @@
         <v>1527.01055414283</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5">
+        <v>0.314</v>
+      </c>
+      <c r="F5">
+        <f>ABS(E5-(32.3300000000003/100))</f>
+        <v>9.3000000000029726E-3</v>
+      </c>
+      <c r="G5">
+        <f>ABS(E5-(30.46/100))</f>
+        <v>9.4000000000000195E-3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5">
+        <f>F5</f>
+        <v>9.3000000000029726E-3</v>
+      </c>
+      <c r="J5">
+        <f>G5</f>
+        <v>9.4000000000000195E-3</v>
+      </c>
+      <c r="K5">
+        <v>1524.58055056373</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <f>K5+2*L5</f>
+        <v>1526.58055056373</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <v>73.3</v>
+      </c>
+      <c r="C6">
+        <f>ABS(B6-73.4100000000017)</f>
+        <v>0.11000000000170473</v>
+      </c>
+      <c r="D6">
+        <f>ABS(B6-73.1800000000016)</f>
+        <v>0.11999999999839872</v>
+      </c>
+      <c r="K6">
+        <v>1523.01684797848</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <f>K6+2*L6</f>
+        <v>1525.01684797848</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7">
+      <c r="B9">
         <v>73.5</v>
       </c>
-      <c r="C7">
+      <c r="C9">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D7">
+      <c r="D9">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E7">
+      <c r="E9">
         <v>0.309</v>
       </c>
-      <c r="F7">
+      <c r="F9">
         <v>6.3E-2</v>
       </c>
-      <c r="G7">
+      <c r="G9">
         <v>-6.9000000000000006E-2</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H9" t="s">
         <v>13</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I9" t="s">
         <v>14</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E8">
+      <c r="E10">
         <v>0.30099999999999999</v>
       </c>
-      <c r="F8">
-        <f>ABS(E8-0.308)</f>
+      <c r="F10">
+        <f>ABS(E10-0.308)</f>
         <v>7.0000000000000062E-3</v>
       </c>
-      <c r="G8">
-        <f>ABS(E8-0.29)</f>
+      <c r="G10">
+        <f>ABS(E10-0.29)</f>
         <v>1.100000000000001E-2</v>
       </c>
-      <c r="H8">
+      <c r="H10">
         <v>-0.92</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I10" t="s">
         <v>16</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J10" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finalisation travail avant vacances hiver
</commit_message>
<xml_diff>
--- a/1_analyse données Pantheon +/restraining parameters/résultats_CL_68_param_cosmo(à compléter).xlsx
+++ b/1_analyse données Pantheon +/restraining parameters/résultats_CL_68_param_cosmo(à compléter).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emile\Desktop\Supaero_3A_2023-2024\projet_recherche\travail_concret_projet\1_analyse données Pantheon +\restraining parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D328114C-2253-40FB-A432-84EC6F761D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3320F673-3AAD-4EDB-9AC1-61D4FF169D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="5865" yWindow="5250" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -133,12 +133,6 @@
     <t>OmegaLambda</t>
   </si>
   <si>
-    <t>Omegam_H0 (pour LambdaCDM)</t>
-  </si>
-  <si>
-    <t>Omegam_Omegal(pour LambdaCDM)</t>
-  </si>
-  <si>
     <t>Résultats attendus pour Flat LCDM (Brout et al. 2022)</t>
   </si>
   <si>
@@ -167,6 +161,12 @@
   </si>
   <si>
     <t>Omegamfixé_H0recherche</t>
+  </si>
+  <si>
+    <t>Omegam_H0 (pour flat LambdaCDM)</t>
+  </si>
+  <si>
+    <t>Omegam_Omegal (attention indroduit de la courbure !)</t>
   </si>
 </sst>
 </file>
@@ -524,7 +524,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,7 +580,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>73.599999999999994</v>
@@ -612,7 +612,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>73.2999999999995</v>
@@ -649,7 +649,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E4">
         <v>0.33</v>
@@ -686,7 +686,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E5">
         <v>0.314</v>
@@ -700,7 +700,7 @@
         <v>9.4000000000000195E-3</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I5">
         <f>F5</f>
@@ -723,7 +723,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>73.3</v>
@@ -749,7 +749,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>73.5</v>
@@ -770,18 +770,18 @@
         <v>-6.9000000000000006E-2</v>
       </c>
       <c r="H9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" t="s">
         <v>13</v>
-      </c>
-      <c r="I9" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E10">
         <v>0.30099999999999999</v>
@@ -798,10 +798,10 @@
         <v>-0.92</v>
       </c>
       <c r="I10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
réorganisation du repo + ajout de nouvelles implémentations de G(z) (→ 1+alpha_m*a)
</commit_message>
<xml_diff>
--- a/1_analyse données Pantheon +/restraining parameters/résultats_CL_68_param_cosmo(à compléter).xlsx
+++ b/1_analyse données Pantheon +/restraining parameters/résultats_CL_68_param_cosmo(à compléter).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emile\Desktop\Supaero_3A_2023-2024\projet_recherche\travail_concret_projet\1_analyse données Pantheon +\restraining parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3320F673-3AAD-4EDB-9AC1-61D4FF169D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F729CA-67D7-442A-BA51-56C9809FD295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="5865" yWindow="5250" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,30 +38,21 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={15528B95-39C7-4CC7-902A-00229DEA6DB7}</author>
-    <author>tc={AF607B9B-BC83-4D48-8FD5-844F9B258B2E}</author>
+    <author>tc={C109FAFE-AFD5-43E1-B207-02F37725EFDF}</author>
     <author>tc={176F64C0-3E19-43A0-A9B6-591B40052657}</author>
     <author>tc={53E0E4B3-50BA-4E72-B223-0D1D050D6508}</author>
     <author>Emile DOSSO</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{15528B95-39C7-4CC7-902A-00229DEA6DB7}">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{C109FAFE-AFD5-43E1-B207-02F37725EFDF}">
       <text>
         <t>[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
-     (sans doute minimisé car range trop petit (s'arrête à 75))</t>
+    Précision meilleure que Brout? Bizarre...</t>
       </text>
     </comment>
-    <comment ref="G3" authorId="1" shapeId="0" xr:uid="{AF607B9B-BC83-4D48-8FD5-844F9B258B2E}">
-      <text>
-        <t>[Commentaire à thread]
-Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
-Commentaire :
-    Meilleure précision que le papier de Brout ! &lt;- cache quelque chose ...</t>
-      </text>
-    </comment>
-    <comment ref="F4" authorId="2" shapeId="0" xr:uid="{176F64C0-3E19-43A0-A9B6-591B40052657}">
+    <comment ref="F5" authorId="1" shapeId="0" xr:uid="{176F64C0-3E19-43A0-A9B6-591B40052657}">
       <text>
         <t>[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
@@ -69,7 +60,7 @@
     (sans doute minimisé car range trop petit (s'arrête à 0.35))</t>
       </text>
     </comment>
-    <comment ref="K4" authorId="3" shapeId="0" xr:uid="{53E0E4B3-50BA-4E72-B223-0D1D050D6508}">
+    <comment ref="K5" authorId="2" shapeId="0" xr:uid="{53E0E4B3-50BA-4E72-B223-0D1D050D6508}">
       <text>
         <t>[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
@@ -77,7 +68,7 @@
     Min de chi2 très similaire à celui pour Omegam_H0 : pourrait être utilisé comme référence pour la suite pour voir si les modèles avec les G(z) améliorent ou non les fits</t>
       </text>
     </comment>
-    <comment ref="G10" authorId="4" shapeId="0" xr:uid="{EB0C4327-299A-426F-82A7-303506DA3CE8}">
+    <comment ref="G11" authorId="3" shapeId="0" xr:uid="{EB0C4327-299A-426F-82A7-303506DA3CE8}">
       <text>
         <r>
           <rPr>
@@ -107,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>+</t>
   </si>
@@ -163,17 +154,23 @@
     <t>Omegamfixé_H0recherche</t>
   </si>
   <si>
-    <t>Omegam_H0 (pour flat LambdaCDM)</t>
-  </si>
-  <si>
     <t>Omegam_Omegal (attention indroduit de la courbure !)</t>
+  </si>
+  <si>
+    <t>Omegam_H0 1.0 avec Omegalambda fixe à 0,666</t>
+  </si>
+  <si>
+    <t>Omegam_H0 2.0 avec Omegalambda = 1 -Omegamatter</t>
+  </si>
+  <si>
+    <t>← référence !</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,6 +190,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -215,9 +219,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -237,7 +242,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Emile DOSSO" id="{5B684DBE-077F-44CE-8336-DBD6409E8451}" userId="S::Emile.DOSSO@student.isae-supaero.fr::83b2e4d5-a8f2-4d73-a6c8-15a2427d0820" providerId="AD"/>
+  <person displayName="Emile" id="{5B684DBE-077F-44CE-8336-DBD6409E8451}" userId="S::Emile.DOSSO@student.isae-supaero.fr::83b2e4d5-a8f2-4d73-a6c8-15a2427d0820" providerId="AD"/>
 </personList>
 </file>
 
@@ -504,16 +509,13 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="C3" dT="2023-12-18T09:19:56.88" personId="{5B684DBE-077F-44CE-8336-DBD6409E8451}" id="{15528B95-39C7-4CC7-902A-00229DEA6DB7}">
-    <text xml:space="preserve"> (sans doute minimisé car range trop petit (s'arrête à 75))</text>
+  <threadedComment ref="C4" dT="2024-02-26T16:52:57.66" personId="{5B684DBE-077F-44CE-8336-DBD6409E8451}" id="{C109FAFE-AFD5-43E1-B207-02F37725EFDF}">
+    <text>Précision meilleure que Brout? Bizarre...</text>
   </threadedComment>
-  <threadedComment ref="G3" dT="2023-12-12T13:12:57.39" personId="{5B684DBE-077F-44CE-8336-DBD6409E8451}" id="{AF607B9B-BC83-4D48-8FD5-844F9B258B2E}">
-    <text>Meilleure précision que le papier de Brout ! &lt;- cache quelque chose ...</text>
-  </threadedComment>
-  <threadedComment ref="F4" dT="2023-12-27T14:11:34.34" personId="{5B684DBE-077F-44CE-8336-DBD6409E8451}" id="{176F64C0-3E19-43A0-A9B6-591B40052657}">
+  <threadedComment ref="F5" dT="2023-12-27T14:11:34.34" personId="{5B684DBE-077F-44CE-8336-DBD6409E8451}" id="{176F64C0-3E19-43A0-A9B6-591B40052657}">
     <text>(sans doute minimisé car range trop petit (s'arrête à 0.35))</text>
   </threadedComment>
-  <threadedComment ref="K4" dT="2023-12-27T14:18:31.21" personId="{5B684DBE-077F-44CE-8336-DBD6409E8451}" id="{53E0E4B3-50BA-4E72-B223-0D1D050D6508}">
+  <threadedComment ref="K5" dT="2023-12-27T14:18:31.21" personId="{5B684DBE-077F-44CE-8336-DBD6409E8451}" id="{53E0E4B3-50BA-4E72-B223-0D1D050D6508}">
     <text>Min de chi2 très similaire à celui pour Omegam_H0 : pourrait être utilisé comme référence pour la suite pour voir si les modèles avec les G(z) améliorent ou non les fits</text>
   </threadedComment>
 </ThreadedComments>
@@ -521,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,9 +540,10 @@
     <col min="11" max="11" width="27" customWidth="1"/>
     <col min="12" max="12" width="21.5703125" customWidth="1"/>
     <col min="13" max="13" width="10.28515625" customWidth="1"/>
+    <col min="14" max="14" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -578,7 +581,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -610,31 +613,32 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>73.2999999999995</v>
       </c>
       <c r="C3">
-        <v>1.7</v>
+        <f>ABS(B3-75.0999999999995)</f>
+        <v>1.7999999999999972</v>
       </c>
       <c r="D3">
-        <f>ABS(B3-(69.5999999999997))</f>
-        <v>3.6999999999998039</v>
+        <f>ABS(B3-(71.5999999999997 ))</f>
+        <v>1.6999999999998039</v>
       </c>
       <c r="E3">
         <f>33.4000000000001/100</f>
         <v>0.33400000000000096</v>
       </c>
       <c r="F3">
-        <f>ABS(E3-(35.0000000000001/100))</f>
-        <v>1.6000000000000014E-2</v>
+        <f>ABS(E3-(37.4000000000001/100))</f>
+        <v>4.0000000000000036E-2</v>
       </c>
       <c r="G3">
-        <f>ABS(E3-(32.5000000000001/100))</f>
-        <v>8.9999999999999525E-3</v>
+        <f>ABS(E3-0.374)</f>
+        <v>3.9999999999999036E-2</v>
       </c>
       <c r="K3">
         <v>1523.01688482443</v>
@@ -647,160 +651,212 @@
         <v>1527.01688482443</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>73.3</v>
+      </c>
+      <c r="C4">
+        <f>ABS(B4-73.6)</f>
+        <v>0.29999999999999716</v>
+      </c>
+      <c r="D4">
+        <f>ABS(B4-73)</f>
+        <v>0.29999999999999716</v>
       </c>
       <c r="E4">
-        <v>0.33</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="F4">
-        <f>ABS(E4-0.35)</f>
-        <v>1.9999999999999962E-2</v>
+        <f>ABS(E4-0.36)</f>
+        <v>2.6999999999999968E-2</v>
       </c>
       <c r="G4">
         <f>ABS(E4-0.306)</f>
-        <v>2.4000000000000021E-2</v>
+        <v>2.7000000000000024E-2</v>
       </c>
       <c r="H4">
-        <v>0.66200000000000003</v>
+        <f>1-E4</f>
+        <v>0.66700000000000004</v>
       </c>
       <c r="I4">
-        <f>ABS(H4-0.694)</f>
-        <v>3.1999999999999917E-2</v>
+        <f>F4</f>
+        <v>2.6999999999999968E-2</v>
       </c>
       <c r="J4">
-        <f>ABS(H4-0.633)</f>
-        <v>2.9000000000000026E-2</v>
+        <f>G4</f>
+        <v>2.7000000000000024E-2</v>
       </c>
       <c r="K4">
-        <v>1523.01055414283</v>
+        <v>1523.0119236576199</v>
       </c>
       <c r="L4">
         <v>2</v>
       </c>
       <c r="M4">
         <f>K4+2*L4</f>
-        <v>1527.01055414283</v>
+        <v>1527.0119236576199</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E5">
-        <v>0.314</v>
+        <v>0.33</v>
       </c>
       <c r="F5">
-        <f>ABS(E5-(32.3300000000003/100))</f>
-        <v>9.3000000000029726E-3</v>
+        <f>ABS(E5-0.35)</f>
+        <v>1.9999999999999962E-2</v>
       </c>
       <c r="G5">
-        <f>ABS(E5-(30.46/100))</f>
-        <v>9.4000000000000195E-3</v>
-      </c>
-      <c r="H5" t="s">
-        <v>16</v>
+        <f>ABS(E5-0.306)</f>
+        <v>2.4000000000000021E-2</v>
+      </c>
+      <c r="H5">
+        <v>0.66200000000000003</v>
       </c>
       <c r="I5">
-        <f>F5</f>
-        <v>9.3000000000029726E-3</v>
+        <f>ABS(H5-0.694)</f>
+        <v>3.1999999999999917E-2</v>
       </c>
       <c r="J5">
-        <f>G5</f>
-        <v>9.4000000000000195E-3</v>
+        <f>ABS(H5-0.633)</f>
+        <v>2.9000000000000026E-2</v>
       </c>
       <c r="K5">
-        <v>1524.58055056373</v>
+        <v>1523.01055414283</v>
       </c>
       <c r="L5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M5">
         <f>K5+2*L5</f>
-        <v>1526.58055056373</v>
+        <v>1527.01055414283</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6">
-        <v>73.3</v>
-      </c>
-      <c r="C6">
-        <f>ABS(B6-73.4100000000017)</f>
-        <v>0.11000000000170473</v>
-      </c>
-      <c r="D6">
-        <f>ABS(B6-73.1800000000016)</f>
-        <v>0.11999999999839872</v>
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>0.314</v>
+      </c>
+      <c r="F6">
+        <f>ABS(E6-(32.3300000000003/100))</f>
+        <v>9.3000000000029726E-3</v>
+      </c>
+      <c r="G6">
+        <f>ABS(E6-(30.46/100))</f>
+        <v>9.4000000000000195E-3</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6">
+        <f>F6</f>
+        <v>9.3000000000029726E-3</v>
+      </c>
+      <c r="J6">
+        <f>G6</f>
+        <v>9.4000000000000195E-3</v>
       </c>
       <c r="K6">
-        <v>1523.01684797848</v>
+        <v>1524.58055056373</v>
       </c>
       <c r="L6">
         <v>1</v>
       </c>
       <c r="M6">
         <f>K6+2*L6</f>
+        <v>1526.58055056373</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>73.3</v>
+      </c>
+      <c r="C7">
+        <f>ABS(B7-73.4100000000017)</f>
+        <v>0.11000000000170473</v>
+      </c>
+      <c r="D7">
+        <f>ABS(B7-73.1800000000016)</f>
+        <v>0.11999999999839872</v>
+      </c>
+      <c r="K7">
+        <v>1523.01684797848</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <f>K7+2*L7</f>
         <v>1525.01684797848</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>73.5</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <v>0.309</v>
       </c>
-      <c r="F9">
+      <c r="F10">
         <v>6.3E-2</v>
       </c>
-      <c r="G9">
+      <c r="G10">
         <v>-6.9000000000000006E-2</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H10" t="s">
         <v>11</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I10" t="s">
         <v>12</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E10">
+      <c r="E11">
         <v>0.30099999999999999</v>
       </c>
-      <c r="F10">
-        <f>ABS(E10-0.308)</f>
+      <c r="F11">
+        <f>ABS(E11-0.308)</f>
         <v>7.0000000000000062E-3</v>
       </c>
-      <c r="G10">
-        <f>ABS(E10-0.29)</f>
+      <c r="G11">
+        <f>ABS(E11-0.29)</f>
         <v>1.100000000000001E-2</v>
       </c>
-      <c r="H10">
+      <c r="H11">
         <v>-0.92</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I11" t="s">
         <v>14</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J11" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>